<commit_message>
refactor: daily excel...change query
</commit_message>
<xml_diff>
--- a/home/static/excel/base.xlsx
+++ b/home/static/excel/base.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="overall" sheetId="4" r:id="rId1"/>
     <sheet name="overall_demographic" sheetId="1" r:id="rId2"/>
     <sheet name="by_course_KPI_honor" sheetId="9" r:id="rId3"/>
-    <sheet name="by_course_KPI_audit" sheetId="2" r:id="rId4"/>
+    <sheet name="by_course_KPI_total" sheetId="2" r:id="rId4"/>
     <sheet name="by_course_demographic_honor" sheetId="3" r:id="rId5"/>
-    <sheet name="by_course_demographic_audit" sheetId="7" r:id="rId6"/>
+    <sheet name="by_course_demographic_total" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">by_course_KPI_audit!$A$3:$AJ$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">by_course_KPI_honor!$A$3:$AJ$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">by_course_KPI_total!$A$3:$AJ$3</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -1102,9 +1102,6 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1112,6 +1109,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1127,10 +1127,10 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2053,25 +2053,25 @@
       <c r="H1" s="16"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="33" t="s">
         <v>25</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="L3" s="10"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="52" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="33" t="s">
@@ -2117,7 +2117,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="33" t="s">
         <v>30</v>
       </c>
@@ -2144,7 +2144,7 @@
       <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="49"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="33" t="s">
         <v>32</v>
       </c>
@@ -2169,7 +2169,7 @@
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="49"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="33" t="s">
         <v>33</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="33" t="s">
         <v>34</v>
       </c>
@@ -2219,7 +2219,7 @@
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="49"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="33" t="s">
         <v>35</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="49"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="34" t="s">
         <v>92</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="2:12" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="33" t="s">
         <v>36</v>
       </c>
@@ -2297,7 +2297,7 @@
       <c r="J11" s="31"/>
     </row>
     <row r="12" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="52" t="s">
         <v>81</v>
       </c>
       <c r="C12" s="33" t="s">
@@ -2323,7 +2323,7 @@
       <c r="L12" s="10"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="33" t="s">
         <v>30</v>
       </c>
@@ -2350,7 +2350,7 @@
       <c r="L13" s="10"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="49"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="33" t="s">
         <v>32</v>
       </c>
@@ -2375,7 +2375,7 @@
       <c r="L14" s="10"/>
     </row>
     <row r="15" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="49"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="33" t="s">
         <v>33</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="L15" s="10"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="49"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="33" t="s">
         <v>34</v>
       </c>
@@ -2425,7 +2425,7 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="49"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="33" t="s">
         <v>35</v>
       </c>
@@ -2450,7 +2450,7 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="49"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="34" t="s">
         <v>92</v>
       </c>
@@ -2475,7 +2475,7 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="2:12" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="49"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="33" t="s">
         <v>36</v>
       </c>
@@ -2503,7 +2503,7 @@
       <c r="J19" s="31"/>
     </row>
     <row r="20" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="52" t="s">
         <v>83</v>
       </c>
       <c r="C20" s="33" t="s">
@@ -2529,7 +2529,7 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="49"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="33" t="s">
         <v>30</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="49"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="33" t="s">
         <v>32</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="L22" s="10"/>
     </row>
     <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="49"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="33" t="s">
         <v>33</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="L23" s="10"/>
     </row>
     <row r="24" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="49"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="33" t="s">
         <v>34</v>
       </c>
@@ -2631,7 +2631,7 @@
       <c r="L24" s="10"/>
     </row>
     <row r="25" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="49"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="33" t="s">
         <v>35</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="L25" s="10"/>
     </row>
     <row r="26" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="49"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="34" t="s">
         <v>92</v>
       </c>
@@ -2681,7 +2681,7 @@
       <c r="L26" s="10"/>
     </row>
     <row r="27" spans="2:12" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="49"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="33" t="s">
         <v>36</v>
       </c>
@@ -2709,7 +2709,7 @@
       <c r="J27" s="31"/>
     </row>
     <row r="28" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="52" t="s">
         <v>79</v>
       </c>
       <c r="C28" s="33" t="s">
@@ -2735,7 +2735,7 @@
       <c r="L28" s="10"/>
     </row>
     <row r="29" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="49"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="33" t="s">
         <v>30</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="L29" s="10"/>
     </row>
     <row r="30" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="49"/>
+      <c r="B30" s="52"/>
       <c r="C30" s="33" t="s">
         <v>32</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="L30" s="10"/>
     </row>
     <row r="31" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="49"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="33" t="s">
         <v>33</v>
       </c>
@@ -2812,7 +2812,7 @@
       <c r="L31" s="10"/>
     </row>
     <row r="32" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="49"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="33" t="s">
         <v>34</v>
       </c>
@@ -2837,7 +2837,7 @@
       <c r="L32" s="10"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="49"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="33" t="s">
         <v>35</v>
       </c>
@@ -2862,7 +2862,7 @@
       <c r="L33" s="10"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="49"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="34" t="s">
         <v>92</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="L34" s="10"/>
     </row>
     <row r="35" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="49"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="33" t="s">
         <v>36</v>
       </c>
@@ -2940,17 +2940,17 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51" t="s">
+      <c r="C38" s="49"/>
+      <c r="D38" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
@@ -2958,8 +2958,8 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="33" t="s">
         <v>25</v>
       </c>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="52" t="s">
         <v>80</v>
       </c>
       <c r="C40" s="33" t="s">
@@ -3011,7 +3011,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="49"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="33" t="s">
         <v>38</v>
       </c>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="49"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="33" t="s">
         <v>39</v>
       </c>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="49"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="33" t="s">
         <v>40</v>
       </c>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="49"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="33" t="s">
         <v>41</v>
       </c>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="49"/>
+      <c r="B45" s="52"/>
       <c r="C45" s="33" t="s">
         <v>42</v>
       </c>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
-      <c r="B46" s="49"/>
+      <c r="B46" s="52"/>
       <c r="C46" s="33" t="s">
         <v>43</v>
       </c>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="49"/>
+      <c r="B47" s="52"/>
       <c r="C47" s="33" t="s">
         <v>27</v>
       </c>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="49"/>
+      <c r="B48" s="52"/>
       <c r="C48" s="33" t="s">
         <v>44</v>
       </c>
@@ -3226,7 +3226,7 @@
       <c r="L48" s="10"/>
     </row>
     <row r="49" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="49"/>
+      <c r="B49" s="52"/>
       <c r="C49" s="33" t="s">
         <v>36</v>
       </c>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="49" t="s">
+      <c r="B50" s="52" t="s">
         <v>81</v>
       </c>
       <c r="C50" s="33" t="s">
@@ -3282,7 +3282,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="49"/>
+      <c r="B51" s="52"/>
       <c r="C51" s="33" t="s">
         <v>38</v>
       </c>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
-      <c r="B52" s="49"/>
+      <c r="B52" s="52"/>
       <c r="C52" s="33" t="s">
         <v>39</v>
       </c>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="49"/>
+      <c r="B53" s="52"/>
       <c r="C53" s="33" t="s">
         <v>40</v>
       </c>
@@ -3363,7 +3363,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="49"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="33" t="s">
         <v>41</v>
       </c>
@@ -3390,7 +3390,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="49"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="33" t="s">
         <v>42</v>
       </c>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
-      <c r="B56" s="49"/>
+      <c r="B56" s="52"/>
       <c r="C56" s="33" t="s">
         <v>43</v>
       </c>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
-      <c r="B57" s="49"/>
+      <c r="B57" s="52"/>
       <c r="C57" s="33" t="s">
         <v>27</v>
       </c>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
-      <c r="B58" s="49"/>
+      <c r="B58" s="52"/>
       <c r="C58" s="33" t="s">
         <v>44</v>
       </c>
@@ -3497,7 +3497,7 @@
       <c r="L58" s="10"/>
     </row>
     <row r="59" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="49"/>
+      <c r="B59" s="52"/>
       <c r="C59" s="33" t="s">
         <v>36</v>
       </c>
@@ -3524,7 +3524,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
-      <c r="B60" s="49" t="s">
+      <c r="B60" s="52" t="s">
         <v>85</v>
       </c>
       <c r="C60" s="33" t="s">
@@ -3553,7 +3553,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
-      <c r="B61" s="49"/>
+      <c r="B61" s="52"/>
       <c r="C61" s="33" t="s">
         <v>38</v>
       </c>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
-      <c r="B62" s="49"/>
+      <c r="B62" s="52"/>
       <c r="C62" s="33" t="s">
         <v>39</v>
       </c>
@@ -3607,7 +3607,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
-      <c r="B63" s="49"/>
+      <c r="B63" s="52"/>
       <c r="C63" s="33" t="s">
         <v>40</v>
       </c>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
-      <c r="B64" s="49"/>
+      <c r="B64" s="52"/>
       <c r="C64" s="33" t="s">
         <v>41</v>
       </c>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
-      <c r="B65" s="49"/>
+      <c r="B65" s="52"/>
       <c r="C65" s="33" t="s">
         <v>42</v>
       </c>
@@ -3688,7 +3688,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
-      <c r="B66" s="49"/>
+      <c r="B66" s="52"/>
       <c r="C66" s="33" t="s">
         <v>43</v>
       </c>
@@ -3715,7 +3715,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
-      <c r="B67" s="49"/>
+      <c r="B67" s="52"/>
       <c r="C67" s="33" t="s">
         <v>27</v>
       </c>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
-      <c r="B68" s="49"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="33" t="s">
         <v>44</v>
       </c>
@@ -3768,7 +3768,7 @@
       <c r="L68" s="10"/>
     </row>
     <row r="69" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="49"/>
+      <c r="B69" s="52"/>
       <c r="C69" s="33" t="s">
         <v>36</v>
       </c>
@@ -3795,7 +3795,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
-      <c r="B70" s="49" t="s">
+      <c r="B70" s="52" t="s">
         <v>82</v>
       </c>
       <c r="C70" s="33" t="s">
@@ -3824,7 +3824,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
-      <c r="B71" s="49"/>
+      <c r="B71" s="52"/>
       <c r="C71" s="33" t="s">
         <v>38</v>
       </c>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
-      <c r="B72" s="49"/>
+      <c r="B72" s="52"/>
       <c r="C72" s="33" t="s">
         <v>39</v>
       </c>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
-      <c r="B73" s="49"/>
+      <c r="B73" s="52"/>
       <c r="C73" s="33" t="s">
         <v>40</v>
       </c>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
-      <c r="B74" s="49"/>
+      <c r="B74" s="52"/>
       <c r="C74" s="33" t="s">
         <v>41</v>
       </c>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
-      <c r="B75" s="49"/>
+      <c r="B75" s="52"/>
       <c r="C75" s="33" t="s">
         <v>42</v>
       </c>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
-      <c r="B76" s="49"/>
+      <c r="B76" s="52"/>
       <c r="C76" s="33" t="s">
         <v>43</v>
       </c>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
-      <c r="B77" s="49"/>
+      <c r="B77" s="52"/>
       <c r="C77" s="33" t="s">
         <v>27</v>
       </c>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
-      <c r="B78" s="49"/>
+      <c r="B78" s="52"/>
       <c r="C78" s="33" t="s">
         <v>44</v>
       </c>
@@ -4039,7 +4039,7 @@
       <c r="L78" s="10"/>
     </row>
     <row r="79" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="49"/>
+      <c r="B79" s="52"/>
       <c r="C79" s="33" t="s">
         <v>36</v>
       </c>
@@ -4090,27 +4090,27 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
-      <c r="B82" s="51" t="s">
+      <c r="B82" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C82" s="51"/>
-      <c r="D82" s="51" t="s">
+      <c r="C82" s="50"/>
+      <c r="D82" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E82" s="52"/>
-      <c r="F82" s="52"/>
-      <c r="G82" s="52"/>
-      <c r="H82" s="52"/>
-      <c r="I82" s="52"/>
-      <c r="J82" s="52"/>
-      <c r="K82" s="52"/>
-      <c r="L82" s="52"/>
-      <c r="M82" s="52"/>
+      <c r="E82" s="51"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="51"/>
+      <c r="I82" s="51"/>
+      <c r="J82" s="51"/>
+      <c r="K82" s="51"/>
+      <c r="L82" s="51"/>
+      <c r="M82" s="51"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
-      <c r="B83" s="51"/>
-      <c r="C83" s="51"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="50"/>
       <c r="D83" s="33" t="s">
         <v>37</v>
       </c>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
-      <c r="B84" s="49" t="s">
+      <c r="B84" s="52" t="s">
         <v>80</v>
       </c>
       <c r="C84" s="29" t="s">
@@ -4184,7 +4184,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
-      <c r="B85" s="49"/>
+      <c r="B85" s="52"/>
       <c r="C85" s="29" t="s">
         <v>30</v>
       </c>
@@ -4221,7 +4221,7 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B86" s="49"/>
+      <c r="B86" s="52"/>
       <c r="C86" s="29" t="s">
         <v>32</v>
       </c>
@@ -4258,7 +4258,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B87" s="49"/>
+      <c r="B87" s="52"/>
       <c r="C87" s="29" t="s">
         <v>33</v>
       </c>
@@ -4295,7 +4295,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B88" s="49"/>
+      <c r="B88" s="52"/>
       <c r="C88" s="29" t="s">
         <v>34</v>
       </c>
@@ -4333,7 +4333,7 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
-      <c r="B89" s="49"/>
+      <c r="B89" s="52"/>
       <c r="C89" s="29" t="s">
         <v>35</v>
       </c>
@@ -4371,7 +4371,7 @@
     </row>
     <row r="90" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
-      <c r="B90" s="49"/>
+      <c r="B90" s="52"/>
       <c r="C90" s="29" t="s">
         <v>90</v>
       </c>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="91" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11"/>
-      <c r="B91" s="49"/>
+      <c r="B91" s="52"/>
       <c r="C91" s="29" t="s">
         <v>36</v>
       </c>
@@ -4456,7 +4456,7 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
-      <c r="B92" s="49" t="s">
+      <c r="B92" s="52" t="s">
         <v>81</v>
       </c>
       <c r="C92" s="29" t="s">
@@ -4496,7 +4496,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
-      <c r="B93" s="49"/>
+      <c r="B93" s="52"/>
       <c r="C93" s="29" t="s">
         <v>30</v>
       </c>
@@ -4533,7 +4533,7 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B94" s="49"/>
+      <c r="B94" s="52"/>
       <c r="C94" s="29" t="s">
         <v>32</v>
       </c>
@@ -4570,7 +4570,7 @@
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B95" s="49"/>
+      <c r="B95" s="52"/>
       <c r="C95" s="29" t="s">
         <v>33</v>
       </c>
@@ -4607,7 +4607,7 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B96" s="49"/>
+      <c r="B96" s="52"/>
       <c r="C96" s="29" t="s">
         <v>34</v>
       </c>
@@ -4645,7 +4645,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
-      <c r="B97" s="49"/>
+      <c r="B97" s="52"/>
       <c r="C97" s="29" t="s">
         <v>35</v>
       </c>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="98" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11"/>
-      <c r="B98" s="49"/>
+      <c r="B98" s="52"/>
       <c r="C98" s="29" t="s">
         <v>90</v>
       </c>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="99" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11"/>
-      <c r="B99" s="49"/>
+      <c r="B99" s="52"/>
       <c r="C99" s="29" t="s">
         <v>36</v>
       </c>
@@ -4768,7 +4768,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
-      <c r="B100" s="49" t="s">
+      <c r="B100" s="52" t="s">
         <v>83</v>
       </c>
       <c r="C100" s="29" t="s">
@@ -4808,7 +4808,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
-      <c r="B101" s="49"/>
+      <c r="B101" s="52"/>
       <c r="C101" s="29" t="s">
         <v>30</v>
       </c>
@@ -4845,7 +4845,7 @@
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B102" s="49"/>
+      <c r="B102" s="52"/>
       <c r="C102" s="29" t="s">
         <v>32</v>
       </c>
@@ -4882,7 +4882,7 @@
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B103" s="49"/>
+      <c r="B103" s="52"/>
       <c r="C103" s="29" t="s">
         <v>33</v>
       </c>
@@ -4919,7 +4919,7 @@
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B104" s="49"/>
+      <c r="B104" s="52"/>
       <c r="C104" s="29" t="s">
         <v>34</v>
       </c>
@@ -4957,7 +4957,7 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
-      <c r="B105" s="49"/>
+      <c r="B105" s="52"/>
       <c r="C105" s="29" t="s">
         <v>35</v>
       </c>
@@ -4995,7 +4995,7 @@
     </row>
     <row r="106" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="11"/>
-      <c r="B106" s="49"/>
+      <c r="B106" s="52"/>
       <c r="C106" s="29" t="s">
         <v>90</v>
       </c>
@@ -5033,7 +5033,7 @@
     </row>
     <row r="107" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11"/>
-      <c r="B107" s="49"/>
+      <c r="B107" s="52"/>
       <c r="C107" s="29" t="s">
         <v>36</v>
       </c>
@@ -5079,7 +5079,7 @@
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B108" s="49" t="s">
+      <c r="B108" s="52" t="s">
         <v>82</v>
       </c>
       <c r="C108" s="29" t="s">
@@ -5118,7 +5118,7 @@
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B109" s="49"/>
+      <c r="B109" s="52"/>
       <c r="C109" s="29" t="s">
         <v>30</v>
       </c>
@@ -5155,7 +5155,7 @@
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B110" s="49"/>
+      <c r="B110" s="52"/>
       <c r="C110" s="29" t="s">
         <v>32</v>
       </c>
@@ -5192,7 +5192,7 @@
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B111" s="49"/>
+      <c r="B111" s="52"/>
       <c r="C111" s="29" t="s">
         <v>33</v>
       </c>
@@ -5229,7 +5229,7 @@
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B112" s="49"/>
+      <c r="B112" s="52"/>
       <c r="C112" s="29" t="s">
         <v>34</v>
       </c>
@@ -5266,7 +5266,7 @@
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B113" s="49"/>
+      <c r="B113" s="52"/>
       <c r="C113" s="29" t="s">
         <v>35</v>
       </c>
@@ -5304,7 +5304,7 @@
     </row>
     <row r="114" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="11"/>
-      <c r="B114" s="49"/>
+      <c r="B114" s="52"/>
       <c r="C114" s="29" t="s">
         <v>90</v>
       </c>
@@ -5342,7 +5342,7 @@
     </row>
     <row r="115" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11"/>
-      <c r="B115" s="49"/>
+      <c r="B115" s="52"/>
       <c r="C115" s="29" t="s">
         <v>36</v>
       </c>
@@ -5389,6 +5389,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B108:B115"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="B92:B99"/>
+    <mergeCell ref="B100:B107"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="B20:B27"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="D82:M82"/>
     <mergeCell ref="B40:B49"/>
@@ -5400,13 +5407,6 @@
     <mergeCell ref="D38:H38"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="B82:C83"/>
-    <mergeCell ref="B108:B115"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="B92:B99"/>
-    <mergeCell ref="B100:B107"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="B20:B27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
@@ -5465,24 +5465,24 @@
       <c r="L1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
       <c r="R1" s="44"/>
       <c r="S1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
       <c r="W1" s="42"/>
       <c r="X1" s="39" t="s">
         <v>22</v>
       </c>
       <c r="Y1" s="44"/>
-      <c r="Z1" s="50" t="s">
+      <c r="Z1" s="49" t="s">
         <v>48</v>
       </c>
       <c r="AA1" s="11"/>
@@ -5509,11 +5509,11 @@
       <c r="J2" s="56"/>
       <c r="K2" s="57"/>
       <c r="L2" s="45"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
       <c r="R2" s="46"/>
       <c r="S2" s="39" t="s">
         <v>4</v>
@@ -5528,7 +5528,7 @@
       </c>
       <c r="X2" s="45"/>
       <c r="Y2" s="46"/>
-      <c r="Z2" s="58"/>
+      <c r="Z2" s="61"/>
     </row>
     <row r="3" spans="1:36" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -5628,7 +5628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -5675,24 +5675,24 @@
       <c r="L1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
       <c r="R1" s="44"/>
       <c r="S1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
       <c r="W1" s="42"/>
       <c r="X1" s="39" t="s">
         <v>22</v>
       </c>
       <c r="Y1" s="44"/>
-      <c r="Z1" s="50" t="s">
+      <c r="Z1" s="49" t="s">
         <v>48</v>
       </c>
       <c r="AA1" s="11"/>
@@ -5719,11 +5719,11 @@
       <c r="J2" s="56"/>
       <c r="K2" s="57"/>
       <c r="L2" s="45"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
       <c r="R2" s="46"/>
       <c r="S2" s="39" t="s">
         <v>4</v>
@@ -5738,7 +5738,7 @@
       </c>
       <c r="X2" s="45"/>
       <c r="Y2" s="46"/>
-      <c r="Z2" s="58"/>
+      <c r="Z2" s="61"/>
     </row>
     <row r="3" spans="1:36" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -6290,11 +6290,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="V2:AD2"/>
-    <mergeCell ref="L1:AE1"/>
-    <mergeCell ref="L2:O2"/>
     <mergeCell ref="AF1:AY1"/>
     <mergeCell ref="AJ2:AO2"/>
     <mergeCell ref="AP2:AX2"/>
@@ -6303,6 +6298,11 @@
     <mergeCell ref="BD2:BI2"/>
     <mergeCell ref="BJ2:BR2"/>
     <mergeCell ref="AZ2:BC2"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="V2:AD2"/>
+    <mergeCell ref="L1:AE1"/>
+    <mergeCell ref="L2:O2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6313,7 +6313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>

</xml_diff>